<commit_message>
Added roc-auc & FP/FN/TP/TN scores to results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B\Desktop\Uni\PhD\Physical\Project\False-Data-Injection-Detection-for-Smart-Grid-Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469C9FFA-CE89-431A-B3A4-61CF178F693F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80D132C-1661-438D-AEED-591B376348A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{DB13A7B6-A9F6-44BD-A24F-2A24EF4BD986}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB13A7B6-A9F6-44BD-A24F-2A24EF4BD986}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Accuracy</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>F1Score1</t>
+  </si>
+  <si>
+    <t>TP Rate</t>
+  </si>
+  <si>
+    <t>FN Rate</t>
+  </si>
+  <si>
+    <t>TN Rate</t>
+  </si>
+  <si>
+    <t>FP Rate</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROC AUC </t>
   </si>
 </sst>
 </file>
@@ -1201,6 +1219,1000 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>initial!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROC AUC </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>initial!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Random Forect</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GaussianNB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KNeighborsClassifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GradientBoosting</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Bagging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>initial!$B$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.97399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55900000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.50600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E60-40F1-8CCE-9EC84D48EDE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="789187359"/>
+        <c:axId val="789189855"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="789187359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="789189855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="789189855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="789187359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Confusion Matrix Rates</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TP Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>initial!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Random Forect</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GaussianNB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KNeighborsClassifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GradientBoosting</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Bagging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>initial!$B$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44F7-44F0-AC71-C432C1BB2BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FN Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>initial!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Random Forect</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GaussianNB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KNeighborsClassifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GradientBoosting</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Bagging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>initial!$B$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-44F7-44F0-AC71-C432C1BB2BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FP Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>initial!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Random Forect</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GaussianNB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KNeighborsClassifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GradientBoosting</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Bagging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>initial!$B$13:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-44F7-44F0-AC71-C432C1BB2BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TN Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>initial!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Random Forect</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GaussianNB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KNeighborsClassifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AdaBoost</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GradientBoosting</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Bagging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>initial!$B$14:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.78600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-44F7-44F0-AC71-C432C1BB2BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="831099695"/>
+        <c:axId val="831104271"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="831099695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="831104271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="831104271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="831099695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>scaled!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1462,7 +2474,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2298,6 +3310,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3808,7 +4900,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4012,6 +5104,1014 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -4314,16 +6414,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>862012</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4350,15 +6450,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>852487</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>338137</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4379,6 +6479,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{225DFA58-53DB-4CC3-96F4-7F401A95B512}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C204315-6211-47D8-ACCE-6EFA104D0DE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4761,10 +6933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF88E30-9087-4055-8DE5-F47D62670C56}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5034,6 +7206,166 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="E10">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="F10">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H10">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I10">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="F11">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="G11">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H11">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="I11">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>0.214</v>
+      </c>
+      <c r="C13">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="F13">
+        <v>0.438</v>
+      </c>
+      <c r="G13">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="H13">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="I13">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="J13">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="C14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D14">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E14">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="G14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.106</v>
+      </c>
+      <c r="I14">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J14">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5045,7 +7377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3268192-9544-431F-9349-D487156342F4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
K-Fold cross validation testing
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B\Desktop\Uni\PhD\Physical\Project\False-Data-Injection-Detection-for-Smart-Grid-Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brenn\Documents\School\M.A.Sc\CISC 850\False-Data-Injection-Detection-for-Smart-Grid-Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80D132C-1661-438D-AEED-591B376348A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B344D95-DF10-49EB-BBC5-55886BAE9A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB13A7B6-A9F6-44BD-A24F-2A24EF4BD986}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DB13A7B6-A9F6-44BD-A24F-2A24EF4BD986}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
     <sheet name="scaled" sheetId="2" r:id="rId2"/>
+    <sheet name="10-Fold" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Accuracy</t>
   </si>
@@ -102,6 +103,15 @@
   </si>
   <si>
     <t xml:space="preserve">ROC AUC </t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>Training Time(s)</t>
+  </si>
+  <si>
+    <t>Testing Time(s)</t>
   </si>
 </sst>
 </file>
@@ -6933,27 +6943,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF88E30-9087-4055-8DE5-F47D62670C56}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6982,7 +6992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7014,7 +7024,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -7046,7 +7056,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -7078,7 +7088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -7110,7 +7120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -7142,7 +7152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -7174,7 +7184,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -7206,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -7238,7 +7248,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -7270,7 +7280,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -7302,7 +7312,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -7334,7 +7344,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -7364,6 +7374,70 @@
       </c>
       <c r="J14">
         <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="C16">
+        <v>346.7</v>
+      </c>
+      <c r="D16">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.03</v>
+      </c>
+      <c r="G16">
+        <v>0.62</v>
+      </c>
+      <c r="H16">
+        <v>10.92</v>
+      </c>
+      <c r="I16">
+        <v>52.74</v>
+      </c>
+      <c r="J16">
+        <v>265.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>0.44</v>
+      </c>
+      <c r="C17">
+        <v>9.77</v>
+      </c>
+      <c r="D17">
+        <v>0.02</v>
+      </c>
+      <c r="E17">
+        <v>0.03</v>
+      </c>
+      <c r="F17">
+        <v>7.3</v>
+      </c>
+      <c r="G17">
+        <v>0.02</v>
+      </c>
+      <c r="H17">
+        <v>0.26</v>
+      </c>
+      <c r="I17">
+        <v>0.05</v>
+      </c>
+      <c r="J17">
+        <v>187.96</v>
       </c>
     </row>
   </sheetData>
@@ -7381,21 +7455,21 @@
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -7424,7 +7498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7456,7 +7530,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -7488,7 +7562,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -7520,7 +7594,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -7552,7 +7626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -7584,7 +7658,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -7616,7 +7690,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -7652,4 +7726,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6660C-F940-4C99-8FF5-F26313308248}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.93</v>
+      </c>
+      <c r="D2">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="E2">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F2">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="G2">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="H2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="I2">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="J2">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>317.10000000000002</v>
+      </c>
+      <c r="D4">
+        <v>10.8</v>
+      </c>
+      <c r="E4">
+        <v>1.74</v>
+      </c>
+      <c r="F4">
+        <v>33.1</v>
+      </c>
+      <c r="G4">
+        <v>10.4</v>
+      </c>
+      <c r="H4">
+        <v>194.53</v>
+      </c>
+      <c r="I4">
+        <v>1042.7</v>
+      </c>
+      <c r="J4">
+        <v>7134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>